<commit_message>
working bottom to top slice generator
</commit_message>
<xml_diff>
--- a/docs/input_template_dam.xlsx
+++ b/docs/input_template_dam.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/slopetools/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/CursorProjects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01AC5E6-49D8-8D44-A76D-874CA2CF2449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EE6EAE-DEF4-B84E-9DC4-A59AE5F2111D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4580" yWindow="860" windowWidth="30020" windowHeight="24340" activeTab="3" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="18780" yWindow="780" windowWidth="30020" windowHeight="24340" activeTab="3" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -5020,16 +5020,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="M20:N20"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="M2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5040,7 +5040,7 @@
   <dimension ref="A2:O13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5123,12 +5123,8 @@
       <c r="E4" s="3">
         <v>34</v>
       </c>
-      <c r="F4" s="3">
-        <v>30</v>
-      </c>
-      <c r="G4" s="3">
-        <v>120</v>
-      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
added material name to materials table in input file
</commit_message>
<xml_diff>
--- a/docs/input_template_dam.xlsx
+++ b/docs/input_template_dam.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/CursorProjects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EE6EAE-DEF4-B84E-9DC4-A59AE5F2111D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FDDE6C-7409-A945-A58A-E91008771321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18780" yWindow="780" windowWidth="30020" windowHeight="24340" activeTab="3" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="2800" yWindow="2000" windowWidth="30020" windowHeight="24340" activeTab="3" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="115">
   <si>
     <t>X</t>
   </si>
@@ -95,12 +95,6 @@
   </si>
   <si>
     <t>Profile Line #10</t>
-  </si>
-  <si>
-    <t>Mat</t>
-  </si>
-  <si>
-    <t>Piezo</t>
   </si>
   <si>
     <t>Piezometric Line</t>
@@ -476,6 +470,21 @@
   </si>
   <si>
     <t>Does not move</t>
+  </si>
+  <si>
+    <t>Shell</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>Clay</t>
+  </si>
+  <si>
+    <t>Sand</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -4294,107 +4303,107 @@
   <sheetData>
     <row r="1" spans="1:5" ht="32" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="26" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>20</v>
       </c>
       <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>21</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>23</v>
       </c>
       <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E7" s="24"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="24" t="s">
         <v>26</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>28</v>
       </c>
       <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E9" s="24"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="D10" s="24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E10" s="24"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E11" s="24"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E12" s="24"/>
     </row>
@@ -4406,14 +4415,14 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C16" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D16" s="1">
         <v>62.4</v>
@@ -4421,7 +4430,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C17" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
@@ -4429,7 +4438,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C18" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -4438,7 +4447,7 @@
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
       <c r="C19" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -5020,16 +5029,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="M20:N20"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="M20:N20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5037,196 +5046,212 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA88A0E-2BF5-FE49-9603-08BE4D91829B}">
-  <dimension ref="A2:O13"/>
+  <dimension ref="A2:P13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" style="1" customWidth="1"/>
-    <col min="2" max="8" width="8.5" style="1" customWidth="1"/>
-    <col min="9" max="12" width="8.5" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
+    <col min="3" max="9" width="8.5" style="1" customWidth="1"/>
+    <col min="10" max="13" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B2" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="28"/>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C2" s="28" t="s">
+        <v>86</v>
+      </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
       <c r="F2" s="28"/>
       <c r="G2" s="28"/>
-      <c r="I2" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="J2" s="23"/>
+      <c r="H2" s="28"/>
+      <c r="J2" s="23" t="s">
+        <v>87</v>
+      </c>
       <c r="K2" s="23"/>
-      <c r="L2" s="22"/>
-      <c r="N2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L2" s="23"/>
+      <c r="M2" s="22"/>
+      <c r="O2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="L3" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="3">
         <v>125</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="D4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>34</v>
       </c>
-      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="3">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3">
         <v>1</v>
       </c>
-      <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="N4" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M4" s="3"/>
+      <c r="O4" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="3">
         <v>122</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="D5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="3">
         <v>100</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>26</v>
       </c>
-      <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="3">
+      <c r="H5" s="3"/>
+      <c r="I5" s="3">
         <v>1</v>
       </c>
-      <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="N5" s="1" t="s">
+      <c r="M5" s="3"/>
+      <c r="O5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P5" t="s">
         <v>101</v>
       </c>
-      <c r="O5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="3">
         <v>123</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="D6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="3">
         <v>0</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>24</v>
       </c>
-      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="3">
+      <c r="H6" s="3"/>
+      <c r="I6" s="3">
         <v>1</v>
       </c>
-      <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
-      <c r="N6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="O6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M6" s="3"/>
+      <c r="O6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="P6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="3">
         <v>127</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="D7" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <v>32</v>
       </c>
-      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="3">
+      <c r="H7" s="3"/>
+      <c r="I7" s="3">
         <v>1</v>
       </c>
-      <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -5241,11 +5266,12 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="N8" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M8" s="3"/>
+      <c r="O8" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -5260,14 +5286,15 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="N9" s="1">
+      <c r="M9" s="3"/>
+      <c r="O9" s="1">
         <v>0</v>
       </c>
-      <c r="O9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -5282,14 +5309,15 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="N10" s="1">
+      <c r="M10" s="3"/>
+      <c r="O10" s="1">
         <v>1</v>
       </c>
-      <c r="O10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -5304,9 +5332,10 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M11" s="3"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -5321,9 +5350,10 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M12" s="3"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -5338,37 +5368,38 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="C2:H2"/>
   </mergeCells>
-  <conditionalFormatting sqref="D4:E13">
+  <conditionalFormatting sqref="E4:F13">
     <cfRule type="expression" dxfId="3" priority="5">
-      <formula>$C4="cp"</formula>
+      <formula>$D4="cp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:G13">
+  <conditionalFormatting sqref="G4:H13">
     <cfRule type="expression" dxfId="2" priority="4">
-      <formula>$C4="mc"</formula>
+      <formula>$D4="mc"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4:K13">
+  <conditionalFormatting sqref="K4:L13">
     <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$C4="cp"</formula>
+      <formula>$D4="cp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L4:L13">
+  <conditionalFormatting sqref="M4:M13">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>$C4="mc"</formula>
+      <formula>$D4="mc"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H13" xr:uid="{339A18D9-2C3F-2E47-9927-C099D7AA59DB}">
-      <formula1>$N$9:$N$10</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I13" xr:uid="{339A18D9-2C3F-2E47-9927-C099D7AA59DB}">
+      <formula1>$O$9:$O$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C13" xr:uid="{D6CE31A3-485A-D842-BAD0-54ACE6AD61ED}">
-      <formula1>$N$5:$N$6</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D13" xr:uid="{D6CE31A3-485A-D842-BAD0-54ACE6AD61ED}">
+      <formula1>$O$5:$O$6</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5387,7 +5418,7 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="29"/>
     </row>
@@ -5508,7 +5539,7 @@
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="3">
         <v>182</v>
@@ -5516,34 +5547,34 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="G4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="14" t="s">
+      <c r="J4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="K4" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -5557,7 +5588,7 @@
         <v>500</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E5" s="3">
         <v>197</v>
@@ -5566,10 +5597,10 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="J5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -5583,7 +5614,7 @@
         <v>500</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E6" s="3">
         <v>182</v>
@@ -5592,10 +5623,10 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="J6" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -5610,10 +5641,10 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="J7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K7" t="s">
         <v>96</v>
-      </c>
-      <c r="K7" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -5739,13 +5770,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -5753,10 +5784,10 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
         <v>47</v>
-      </c>
-      <c r="F3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -5764,10 +5795,10 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
         <v>48</v>
-      </c>
-      <c r="F4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -5775,10 +5806,10 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="E5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -5873,22 +5904,22 @@
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
       <c r="F2" s="30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G2" s="30"/>
       <c r="H2" s="30"/>
       <c r="J2" s="30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K2" s="30"/>
       <c r="L2" s="30"/>
       <c r="N2" s="30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="O2" s="30"/>
       <c r="P2" s="30"/>
@@ -5901,7 +5932,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>0</v>
@@ -5910,7 +5941,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>0</v>
@@ -5919,7 +5950,7 @@
         <v>1</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>0</v>
@@ -5928,7 +5959,7 @@
         <v>1</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
@@ -6091,22 +6122,22 @@
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="30" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="30"/>
       <c r="F15" s="30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G15" s="30"/>
       <c r="H15" s="30"/>
       <c r="J15" s="30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K15" s="30"/>
       <c r="L15" s="30"/>
       <c r="N15" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="O15" s="30"/>
       <c r="P15" s="30"/>
@@ -6119,7 +6150,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>0</v>
@@ -6128,7 +6159,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>0</v>
@@ -6137,7 +6168,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>0</v>
@@ -6146,7 +6177,7 @@
         <v>1</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
@@ -6327,25 +6358,25 @@
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B2" s="30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
       <c r="E2" s="30"/>
       <c r="G2" s="30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
       <c r="J2" s="30"/>
       <c r="L2" s="30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M2" s="30"/>
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
       <c r="Q2" s="30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="R2" s="30"/>
       <c r="S2" s="30"/>
@@ -6359,10 +6390,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>0</v>
@@ -6371,10 +6402,10 @@
         <v>1</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>0</v>
@@ -6383,10 +6414,10 @@
         <v>1</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>0</v>
@@ -6395,13 +6426,13 @@
         <v>1</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="V3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.2">
@@ -6422,7 +6453,7 @@
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
       <c r="V4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.2">
@@ -6589,25 +6620,25 @@
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B15" s="30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
       <c r="G15" s="30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H15" s="30"/>
       <c r="I15" s="30"/>
       <c r="J15" s="30"/>
       <c r="L15" s="30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M15" s="30"/>
       <c r="N15" s="30"/>
       <c r="O15" s="30"/>
       <c r="Q15" s="30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R15" s="30"/>
       <c r="S15" s="30"/>
@@ -6621,10 +6652,10 @@
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>0</v>
@@ -6633,10 +6664,10 @@
         <v>1</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>0</v>
@@ -6645,10 +6676,10 @@
         <v>1</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q16" s="2" t="s">
         <v>0</v>
@@ -6657,10 +6688,10 @@
         <v>1</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.2">
@@ -6845,25 +6876,25 @@
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B28" s="30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C28" s="30"/>
       <c r="D28" s="30"/>
       <c r="E28" s="30"/>
       <c r="G28" s="30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H28" s="30"/>
       <c r="I28" s="30"/>
       <c r="J28" s="30"/>
       <c r="L28" s="30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M28" s="30"/>
       <c r="N28" s="30"/>
       <c r="O28" s="30"/>
       <c r="Q28" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R28" s="30"/>
       <c r="S28" s="30"/>
@@ -6877,10 +6908,10 @@
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>0</v>
@@ -6889,10 +6920,10 @@
         <v>1</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>0</v>
@@ -6901,10 +6932,10 @@
         <v>1</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q29" s="2" t="s">
         <v>0</v>
@@ -6913,10 +6944,10 @@
         <v>1</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.2">

</xml_diff>